<commit_message>
completed op & op_imm
</commit_message>
<xml_diff>
--- a/material/Instructions.xlsx
+++ b/material/Instructions.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -285,10 +286,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>I</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -330,6 +327,10 @@
   </si>
   <si>
     <t>SB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -552,17 +553,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -856,7 +857,7 @@
   <dimension ref="B1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="K29" sqref="K29:K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -866,17 +867,17 @@
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.2">
       <c r="H1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="6" t="s">
         <v>1</v>
       </c>
@@ -887,9 +888,9 @@
         <v>2</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>78</v>
       </c>
       <c r="N2" s="2"/>
@@ -913,9 +914,9 @@
         <v>3</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="K3" s="19"/>
+        <v>92</v>
+      </c>
+      <c r="K3" s="16"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
@@ -999,11 +1000,11 @@
       <c r="I6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="K6" s="19" t="s">
-        <v>95</v>
+      <c r="K6" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="L6" s="2"/>
       <c r="N6" s="2"/>
@@ -1032,8 +1033,8 @@
       <c r="I7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
       <c r="L7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1061,8 +1062,8 @@
       <c r="I8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
       <c r="L8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -1090,8 +1091,8 @@
       <c r="I9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1119,8 +1120,8 @@
       <c r="I10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -1148,8 +1149,8 @@
       <c r="I11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
       <c r="L11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1161,7 +1162,7 @@
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
       <c r="E12" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>53</v>
@@ -1175,10 +1176,10 @@
       <c r="I12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="16" t="s">
         <v>81</v>
       </c>
       <c r="L12" s="2"/>
@@ -1206,8 +1207,8 @@
       <c r="I13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -1233,8 +1234,8 @@
       <c r="I14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="18"/>
-      <c r="K14" s="19"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="16"/>
       <c r="L14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -1260,8 +1261,8 @@
       <c r="I15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="18"/>
-      <c r="K15" s="19"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="16"/>
       <c r="L15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -1287,8 +1288,8 @@
       <c r="I16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="K16" s="19"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="16"/>
       <c r="L16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -1316,10 +1317,10 @@
       <c r="I17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="K17" s="19" t="s">
+      <c r="J17" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="K17" s="16" t="s">
         <v>82</v>
       </c>
       <c r="L17" s="2"/>
@@ -1349,8 +1350,8 @@
       <c r="I18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="16"/>
       <c r="L18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -1378,8 +1379,8 @@
       <c r="I19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="16"/>
       <c r="L19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -1405,11 +1406,11 @@
       <c r="I20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J20" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>85</v>
+      <c r="J20" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="L20" s="2"/>
       <c r="N20" s="2"/>
@@ -1417,7 +1418,7 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -1436,8 +1437,8 @@
       <c r="I21" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
       <c r="L21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -1463,8 +1464,8 @@
       <c r="I22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
       <c r="L22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -1490,8 +1491,8 @@
       <c r="I23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
       <c r="L23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -1517,8 +1518,8 @@
       <c r="I24" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
       <c r="L24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -1544,8 +1545,8 @@
       <c r="I25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
       <c r="L25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -1573,8 +1574,8 @@
       <c r="I26" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
       <c r="L26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -1602,8 +1603,8 @@
       <c r="I27" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
       <c r="L27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -1631,8 +1632,8 @@
       <c r="I28" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
       <c r="L28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -1660,11 +1661,11 @@
       <c r="I29" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J29" s="18" t="s">
-        <v>91</v>
+      <c r="J29" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="L29" s="2"/>
       <c r="N29" s="2"/>
@@ -1693,7 +1694,7 @@
       <c r="I30" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J30" s="18"/>
+      <c r="J30" s="17"/>
       <c r="K30" s="21"/>
       <c r="L30" s="2"/>
       <c r="N30" s="2"/>
@@ -1722,7 +1723,7 @@
       <c r="I31" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J31" s="18"/>
+      <c r="J31" s="17"/>
       <c r="K31" s="21"/>
       <c r="L31" s="2"/>
       <c r="N31" s="2"/>
@@ -1751,7 +1752,7 @@
       <c r="I32" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="J32" s="18"/>
+      <c r="J32" s="17"/>
       <c r="K32" s="21"/>
       <c r="L32" s="2"/>
       <c r="N32" s="2"/>
@@ -1780,7 +1781,7 @@
       <c r="I33" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="J33" s="18"/>
+      <c r="J33" s="17"/>
       <c r="K33" s="21"/>
       <c r="L33" s="2"/>
       <c r="N33" s="2"/>
@@ -1809,7 +1810,7 @@
       <c r="I34" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J34" s="18"/>
+      <c r="J34" s="17"/>
       <c r="K34" s="21"/>
       <c r="L34" s="2"/>
       <c r="N34" s="2"/>
@@ -1838,7 +1839,7 @@
       <c r="I35" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J35" s="18"/>
+      <c r="J35" s="17"/>
       <c r="K35" s="21"/>
       <c r="L35" s="2"/>
       <c r="N35" s="2"/>
@@ -1867,7 +1868,7 @@
       <c r="I36" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="J36" s="18"/>
+      <c r="J36" s="17"/>
       <c r="K36" s="21"/>
       <c r="L36" s="2"/>
       <c r="N36" s="2"/>
@@ -1896,7 +1897,7 @@
       <c r="I37" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="J37" s="18"/>
+      <c r="J37" s="17"/>
       <c r="K37" s="21"/>
       <c r="L37" s="2"/>
       <c r="N37" s="2"/>
@@ -1925,7 +1926,7 @@
       <c r="I38" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J38" s="18"/>
+      <c r="J38" s="17"/>
       <c r="K38" s="22"/>
       <c r="L38" s="2"/>
       <c r="N38" s="2"/>
@@ -1956,10 +1957,10 @@
       <c r="I39" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J39" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="K39" s="18" t="s">
+      <c r="J39" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="K39" s="17" t="s">
         <v>83</v>
       </c>
       <c r="L39" s="2"/>
@@ -1991,8 +1992,8 @@
       <c r="I40" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="J40" s="19"/>
-      <c r="K40" s="18"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="17"/>
       <c r="L40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="1"/>
@@ -2069,17 +2070,17 @@
     <mergeCell ref="K6:K11"/>
     <mergeCell ref="K12:K16"/>
     <mergeCell ref="K17:K19"/>
-    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="J6:J11"/>
     <mergeCell ref="J12:J16"/>
     <mergeCell ref="J17:J19"/>
     <mergeCell ref="J20:J28"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
@@ -2088,6 +2089,13 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B26:C26"/>
@@ -2095,20 +2103,13 @@
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B25:D25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>